<commit_message>
change names aaay and aph + precipitation multiplier
</commit_message>
<xml_diff>
--- a/tests/payoutPercentage.xlsx
+++ b/tests/payoutPercentage.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreteves/Solidity/chainlink-hackathon/rainsurance-contracts/gif-contracts-develop/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreteves/Solidity/chainlink-hackathon/rainsurance-contracts/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3085C686-00C6-8D4C-AE71-DA3AE88EF328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311D4C22-C845-6A46-B9D9-181CAE9DC955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{EB52C230-FDD9-CB49-888C-FEB7C6F8F755}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -480,7 +480,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,7 +489,7 @@
     <col min="4" max="5" width="11.1640625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="73.1640625" customWidth="1"/>
+    <col min="8" max="8" width="84.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -511,10 +511,10 @@
       </c>
       <c r="B2" s="5">
         <f>C2*B1</f>
-        <v>12582912</v>
+        <v>838860.80000000005</v>
       </c>
       <c r="C2" s="6">
-        <v>0.75</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -523,10 +523,10 @@
       </c>
       <c r="B3" s="5">
         <f>C3*B1</f>
-        <v>33554432</v>
+        <v>16777216</v>
       </c>
       <c r="C3" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -570,11 +570,11 @@
         <v>0</v>
       </c>
       <c r="E6" s="4">
-        <f>IF(D6=1,$B$1*(C6 - B6) / B6,0)</f>
+        <f t="shared" ref="E6:E27" si="0">IF(D6=1,$B$1*(C6 - B6) / B6,0)</f>
         <v>0</v>
       </c>
       <c r="F6" s="4">
-        <f>IF(E6&lt;=$B$2,1,0)</f>
+        <f t="shared" ref="F6:F27" si="1">IF(E6&lt;=$B$2,1,0)</f>
         <v>1</v>
       </c>
       <c r="G6" s="4">
@@ -582,8 +582,8 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="str">
-        <f>"assert get_payout_delta("&amp;G6&amp;", aph, "&amp;C6&amp;", trigger, exit, product, multiplier) &lt; 0.000001"</f>
-        <v>assert get_payout_delta(0, aph, 0, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f>"assert get_payout_delta("&amp;G6&amp;", aph, "&amp;C6&amp;", trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001"</f>
+        <v>assert get_payout_delta(0, aph, 0, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -591,30 +591,31 @@
         <v>2</v>
       </c>
       <c r="B7" s="4">
+        <f>B6</f>
         <v>5</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" ref="D7:D26" si="0">IF(C7&lt;=B7,0,1)</f>
+        <f t="shared" ref="D7:D26" si="2">IF(C7&lt;=B7,0,1)</f>
         <v>0</v>
       </c>
       <c r="E7" s="4">
-        <f>IF(D7=1,$B$1*(C7 - B7) / B7,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7" s="4">
-        <f>IF(E7&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" ref="G7:G26" si="1">IF(F7=1,0,MIN($B$1,$B$1*E7/$B$3)/$B$1)</f>
+        <f t="shared" ref="G7:G26" si="3">IF(F7=1,0,MIN($B$1,$B$1*E7/$B$3)/$B$1)</f>
         <v>0</v>
       </c>
       <c r="H7" s="5" t="str">
-        <f t="shared" ref="H7:H27" si="2">"assert get_payout_delta("&amp;G7&amp;", aph, "&amp;C7&amp;", trigger, exit, product, multiplier) &lt; 0.000001"</f>
-        <v>assert get_payout_delta(0, aph, 1, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" ref="H7:H27" si="4">"assert get_payout_delta("&amp;G7&amp;", aph, "&amp;C7&amp;", trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001"</f>
+        <v>assert get_payout_delta(0, aph, 1, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -622,6 +623,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="4">
+        <f t="shared" ref="B8:B26" si="5">B7</f>
         <v>5</v>
       </c>
       <c r="C8" s="4">
@@ -629,24 +631,24 @@
         <v>2</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E8" s="4">
-        <f>IF(D8=1,$B$1*(C8 - B8) / B8,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <f>IF(E8&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H8" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0, aph, 2, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(0, aph, 2, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -654,31 +656,32 @@
         <v>4</v>
       </c>
       <c r="B9" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" ref="C9:C26" si="3">C8+1</f>
+        <f t="shared" ref="C9:C26" si="6">C8+1</f>
         <v>3</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E9" s="4">
-        <f>IF(D9=1,$B$1*(C9 - B9) / B9,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="4">
-        <f>IF(E9&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H9" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0, aph, 3, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(0, aph, 3, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -686,31 +689,32 @@
         <v>5</v>
       </c>
       <c r="B10" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E10" s="4">
-        <f>IF(D10=1,$B$1*(C10 - B10) / B10,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10" s="4">
-        <f>IF(E10&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H10" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0, aph, 4, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(0, aph, 4, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -718,31 +722,32 @@
         <v>6</v>
       </c>
       <c r="B11" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E11" s="4">
-        <f>IF(D11=1,$B$1*(C11 - B11) / B11,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" s="4">
-        <f>IF(E11&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H11" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0, aph, 5, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(0, aph, 5, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -750,31 +755,32 @@
         <v>7</v>
       </c>
       <c r="B12" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E12" s="4">
-        <f>IF(D12=1,$B$1*(C12 - B12) / B12,0)</f>
+        <f t="shared" si="0"/>
         <v>3355443.2000000002</v>
       </c>
       <c r="F12" s="4">
-        <f>IF(E12&lt;=$B$2,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.2</v>
       </c>
       <c r="H12" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0, aph, 6, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(0,2, aph, 6, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -782,31 +788,32 @@
         <v>8</v>
       </c>
       <c r="B13" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E13" s="4">
-        <f>IF(D13=1,$B$1*(C13 - B13) / B13,0)</f>
+        <f t="shared" si="0"/>
         <v>6710886.4000000004</v>
       </c>
       <c r="F13" s="4">
-        <f>IF(E13&lt;=$B$2,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.4</v>
       </c>
       <c r="H13" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0, aph, 7, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(0,4, aph, 7, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -814,31 +821,32 @@
         <v>9</v>
       </c>
       <c r="B14" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E14" s="4">
-        <f>IF(D14=1,$B$1*(C14 - B14) / B14,0)</f>
+        <f t="shared" si="0"/>
         <v>10066329.6</v>
       </c>
       <c r="F14" s="4">
-        <f>IF(E14&lt;=$B$2,1,0)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.6</v>
       </c>
       <c r="H14" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0, aph, 8, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(0,6, aph, 8, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -846,31 +854,32 @@
         <v>10</v>
       </c>
       <c r="B15" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E15" s="4">
-        <f>IF(D15=1,$B$1*(C15 - B15) / B15,0)</f>
+        <f t="shared" si="0"/>
         <v>13421772.800000001</v>
       </c>
       <c r="F15" s="4">
-        <f>IF(E15&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
+        <f t="shared" si="3"/>
+        <v>0.8</v>
       </c>
       <c r="H15" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0,4, aph, 9, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(0,8, aph, 9, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -878,31 +887,32 @@
         <v>11</v>
       </c>
       <c r="B16" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C16" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E16" s="4">
-        <f>IF(D16=1,$B$1*(C16 - B16) / B16,0)</f>
+        <f t="shared" si="0"/>
         <v>16777216</v>
       </c>
       <c r="F16" s="4">
-        <f>IF(E16&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H16" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0,5, aph, 10, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 10, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -910,31 +920,32 @@
         <v>12</v>
       </c>
       <c r="B17" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E17" s="4">
-        <f>IF(D17=1,$B$1*(C17 - B17) / B17,0)</f>
+        <f t="shared" si="0"/>
         <v>20132659.199999999</v>
       </c>
       <c r="F17" s="4">
-        <f>IF(E17&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H17" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0,6, aph, 11, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 11, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -942,31 +953,32 @@
         <v>13</v>
       </c>
       <c r="B18" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E18" s="4">
-        <f>IF(D18=1,$B$1*(C18 - B18) / B18,0)</f>
+        <f t="shared" si="0"/>
         <v>23488102.399999999</v>
       </c>
       <c r="F18" s="4">
-        <f>IF(E18&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="1"/>
-        <v>0.7</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H18" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0,7, aph, 12, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 12, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -974,31 +986,32 @@
         <v>14</v>
       </c>
       <c r="B19" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E19" s="4">
-        <f>IF(D19=1,$B$1*(C19 - B19) / B19,0)</f>
+        <f t="shared" si="0"/>
         <v>26843545.600000001</v>
       </c>
       <c r="F19" s="4">
-        <f>IF(E19&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H19" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0,8, aph, 13, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 13, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1006,31 +1019,32 @@
         <v>15</v>
       </c>
       <c r="B20" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E20" s="4">
-        <f>IF(D20=1,$B$1*(C20 - B20) / B20,0)</f>
+        <f t="shared" si="0"/>
         <v>30198988.800000001</v>
       </c>
       <c r="F20" s="4">
-        <f>IF(E20&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="1"/>
-        <v>0.9</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H20" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0,9, aph, 14, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 14, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1038,31 +1052,32 @@
         <v>16</v>
       </c>
       <c r="B21" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E21" s="4">
-        <f>IF(D21=1,$B$1*(C21 - B21) / B21,0)</f>
+        <f t="shared" si="0"/>
         <v>33554432</v>
       </c>
       <c r="F21" s="4">
-        <f>IF(E21&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H21" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(1, aph, 15, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 15, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1070,31 +1085,32 @@
         <v>17</v>
       </c>
       <c r="B22" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E22" s="4">
-        <f>IF(D22=1,$B$1*(C22 - B22) / B22,0)</f>
+        <f t="shared" si="0"/>
         <v>36909875.200000003</v>
       </c>
       <c r="F22" s="4">
-        <f>IF(E22&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H22" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(1, aph, 16, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 16, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1102,31 +1118,32 @@
         <v>18</v>
       </c>
       <c r="B23" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E23" s="4">
-        <f>IF(D23=1,$B$1*(C23 - B23) / B23,0)</f>
+        <f t="shared" si="0"/>
         <v>40265318.399999999</v>
       </c>
       <c r="F23" s="4">
-        <f>IF(E23&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H23" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(1, aph, 17, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 17, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1134,31 +1151,32 @@
         <v>19</v>
       </c>
       <c r="B24" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E24" s="4">
-        <f>IF(D24=1,$B$1*(C24 - B24) / B24,0)</f>
+        <f t="shared" si="0"/>
         <v>43620761.600000001</v>
       </c>
       <c r="F24" s="4">
-        <f>IF(E24&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H24" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(1, aph, 18, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 18, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1166,31 +1184,32 @@
         <v>20</v>
       </c>
       <c r="B25" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E25" s="4">
-        <f>IF(D25=1,$B$1*(C25 - B25) / B25,0)</f>
+        <f t="shared" si="0"/>
         <v>46976204.799999997</v>
       </c>
       <c r="F25" s="4">
-        <f>IF(E25&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H25" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(1, aph, 19, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 19, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1198,31 +1217,32 @@
         <v>21</v>
       </c>
       <c r="B26" s="4">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E26" s="4">
-        <f>IF(D26=1,$B$1*(C26 - B26) / B26,0)</f>
+        <f t="shared" si="0"/>
         <v>50331648</v>
       </c>
       <c r="F26" s="4">
-        <f>IF(E26&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H26" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(1, aph, 20, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(1, aph, 20, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1230,30 +1250,30 @@
         <v>22</v>
       </c>
       <c r="B27" s="4">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="C27" s="4">
-        <v>4</v>
+        <v>5.88</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" ref="D27" si="4">IF(C27&lt;=B27,0,1)</f>
+        <f t="shared" ref="D27" si="7">IF(C27&lt;=B27,0,1)</f>
         <v>1</v>
       </c>
       <c r="E27" s="4">
-        <f>IF(D27=1,$B$1*(C27 - B27) / B27,0)</f>
-        <v>16777216</v>
+        <f t="shared" si="0"/>
+        <v>6710886.3999999985</v>
       </c>
       <c r="F27" s="4">
-        <f>IF(E27&lt;=$B$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" ref="G27" si="5">IF(F27=1,0,MIN($B$1,$B$1*E27/$B$3)/$B$1)</f>
-        <v>0.5</v>
+        <f t="shared" ref="G27" si="8">IF(F27=1,0,MIN($B$1,$B$1*E27/$B$3)/$B$1)</f>
+        <v>0.39999999999999991</v>
       </c>
       <c r="H27" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>assert get_payout_delta(0,5, aph, 4, trigger, exit, product, multiplier) &lt; 0.000001</v>
+        <f t="shared" si="4"/>
+        <v>assert get_payout_delta(0,4, aph, 5,88, trigger, exit, product, multiplier, precMultiplier) &lt; 0.000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>